<commit_message>
updates to project list + added drawings
</commit_message>
<xml_diff>
--- a/labmanual/project-list.xlsx
+++ b/labmanual/project-list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24340" yWindow="520" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="27200" yWindow="1700" windowWidth="27640" windowHeight="25540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="138">
   <si>
     <t>demo.apollo</t>
   </si>
@@ -146,9 +146,6 @@
     <t>snip.packet_filter</t>
   </si>
   <si>
-    <t>snip.ping_depsleep</t>
-  </si>
-  <si>
     <t>snip.ping_ethernet</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
     <t>6-coap</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
@@ -294,6 +288,156 @@
   </si>
   <si>
     <t>MQTT demonstration of Publisher, Subscriber and Shadow in AWS IOT Cloud</t>
+  </si>
+  <si>
+    <t>Audio demo</t>
+  </si>
+  <si>
+    <t>A BLE based WiFi introducer</t>
+  </si>
+  <si>
+    <t>restful smart server, bluetooth HTTP proxy, blemesh network</t>
+  </si>
+  <si>
+    <t>ble-&gt; http bridge</t>
+  </si>
+  <si>
+    <t>Using COAP to interface with Exosite Cloud</t>
+  </si>
+  <si>
+    <t>A webserver to display the temperature</t>
+  </si>
+  <si>
+    <t>a snip to demonstrate AMQP client</t>
+  </si>
+  <si>
+    <t>a webserver running on an AP displaying the RSSI of the stations(clients) connected</t>
+  </si>
+  <si>
+    <t>run as an Access Point and a Station at the same time</t>
+  </si>
+  <si>
+    <t>streaming audio demo</t>
+  </si>
+  <si>
+    <t>a bluetooth demo</t>
+  </si>
+  <si>
+    <t>This application snippet demonstrates how to react to COAP packet from  network client and activate the services exported by Coap.</t>
+  </si>
+  <si>
+    <t>Start a soft AP to configure the station paramters</t>
+  </si>
+  <si>
+    <t>demonstrate the cryptography library functions</t>
+  </si>
+  <si>
+    <t>A demonstration of read/write of the DCT</t>
+  </si>
+  <si>
+    <t>6-Cloud</t>
+  </si>
+  <si>
+    <t>A demonstation of sending email with SMTP</t>
+  </si>
+  <si>
+    <t>A demonstration of free lossless audio compression</t>
+  </si>
+  <si>
+    <t>read/write pins</t>
+  </si>
+  <si>
+    <t>Display using a U8G display</t>
+  </si>
+  <si>
+    <t>read from an HTTPS server</t>
+  </si>
+  <si>
+    <t>read from HTTPBIN</t>
+  </si>
+  <si>
+    <t>run as an http server</t>
+  </si>
+  <si>
+    <t>demonstrate IPV6</t>
+  </si>
+  <si>
+    <t>demonstrate AP and Station and Ping and webserver</t>
+  </si>
+  <si>
+    <t>snip.ping_deepsleep</t>
+  </si>
+  <si>
+    <t>6-cloud</t>
+  </si>
+  <si>
+    <t>Wifi Protected Setup</t>
+  </si>
+  <si>
+    <t>How to use the UART</t>
+  </si>
+  <si>
+    <t>Simple Service Discovery Protocol</t>
+  </si>
+  <si>
+    <t>use WWD to filter packets</t>
+  </si>
+  <si>
+    <t>use the deepsleep to save power</t>
+  </si>
+  <si>
+    <t>ping using the ethernet interface</t>
+  </si>
+  <si>
+    <t>ping the gateway - display using webserver</t>
+  </si>
+  <si>
+    <t>ping, suspend, low power, resume… do it again</t>
+  </si>
+  <si>
+    <t>Over the air bootloader</t>
+  </si>
+  <si>
+    <t>near field communication</t>
+  </si>
+  <si>
+    <t>demonstate link up/down messages</t>
+  </si>
+  <si>
+    <t>MQTT demo</t>
+  </si>
+  <si>
+    <t>collect and display data about power usage using MAX17040 on the 943907</t>
+  </si>
+  <si>
+    <t>ping, turn off, ping, turn off</t>
+  </si>
+  <si>
+    <t>wwd demo of switching to the best channel</t>
+  </si>
+  <si>
+    <t>scan and display the SSIDs available</t>
+  </si>
+  <si>
+    <t>setup and demonstrate use of STDIO</t>
+  </si>
+  <si>
+    <t>demonstrate MQTT over TLS</t>
+  </si>
+  <si>
+    <t>A big console app that shows all of the capability</t>
+  </si>
+  <si>
+    <t>running wifi performance testing using the iperf protocol</t>
+  </si>
+  <si>
+    <t>nutx nut-sh?</t>
+  </si>
+  <si>
+    <t>a manufacturing test</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -619,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="119" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,10 +790,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,67 +801,109 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -725,400 +911,611 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>46</v>
       </c>
-      <c r="B45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B55" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>57</v>
       </c>
-      <c r="B56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>58</v>
       </c>
-      <c r="B57" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>59</v>
       </c>
-      <c r="B58" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>61</v>
       </c>
-      <c r="B60" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>62</v>
       </c>
-      <c r="B61" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>63</v>
       </c>
-      <c r="B62" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>64</v>
       </c>
-      <c r="B63" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B68" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B70" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>